<commit_message>
Redo asset names, fix building
</commit_message>
<xml_diff>
--- a/Management/Minty-Engine_Working_Hours.xlsx
+++ b/Management/Minty-Engine_Working_Hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitch\source\repos\Minty-Engine\Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitch\Documents\Source\Repos\Minty-Engine\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF6CDCF-A229-4708-969F-D579C534E669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529BA0A0-6C1A-4D8A-AD1B-33CD01722CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="396" windowWidth="23040" windowHeight="12120" activeTab="1" xr2:uid="{D8840A21-015D-4163-9C78-2CDAAC18DA5A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D8840A21-015D-4163-9C78-2CDAAC18DA5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="289">
   <si>
     <t>Start Date</t>
   </si>
@@ -923,6 +923,9 @@
   </si>
   <si>
     <t>Input, Sprites.</t>
+  </si>
+  <si>
+    <t>Building on new device.</t>
   </si>
 </sst>
 </file>
@@ -1389,15 +1392,15 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="6" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="6" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="11" t="s">
         <v>46</v>
@@ -1408,13 +1411,13 @@
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="8">
         <f>SUMIF(Table1[Elapsed Hours], "&gt;0")</f>
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="D2" s="8" t="str">
         <f>ROUNDDOWN($B$2/24, 0) &amp; " days"</f>
@@ -1422,32 +1425,32 @@
       </c>
       <c r="E2" s="10" t="str">
         <f>INT(ROUNDDOWN(MOD($B$2, 24), 0)) &amp; " hours"</f>
-        <v>9 hours</v>
+        <v>11 hours</v>
       </c>
       <c r="F2" s="8" t="str">
         <f>INT(ROUNDDOWN(MOD($B$2,1) * 60,0)) &amp; " minutes"</f>
         <v>0 minutes</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="10">
         <f ca="1">SUMIF(Table1[Start Date],TODAY(),Table1[Elapsed Hours])</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>148</v>
       </c>
       <c r="B4" s="9" cm="1">
         <f t="array" ref="B4">SUMPRODUCT(1/COUNTIF(Table1[[Start Date Value]:[End Date Value]],Table1[[Start Date Value]:[End Date Value]])) - IF(COUNTIF(Table1[[Start Date Value]:[End Date Value]],"&lt;&gt;0")&gt;0,1,0)</f>
-        <v>239.00000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>240.99999999999937</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>206</v>
       </c>
@@ -1456,13 +1459,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>204</v>
       </c>
       <c r="B6" s="9" cm="1">
         <f t="array" ref="B6">_xlfn.XLOOKUP(TRUE,Table1[Streak]&lt;&gt;"",Table1[Streak],,,-1)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1477,20 +1480,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1BE824-2F12-41E9-9B45-9717EA106B41}">
   <dimension ref="A1:K477"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K381" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K393" sqref="K393"/>
+    <sheetView tabSelected="1" topLeftCell="A381" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E395" sqref="E395"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="9" width="18.44140625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1"/>
-    <col min="11" max="11" width="167.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="9" width="18.42578125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="167.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1525,7 +1528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -1805,7 +1808,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1885,7 +1888,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -1925,7 +1928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
@@ -2045,7 +2048,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
@@ -2085,7 +2088,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>8</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
@@ -2165,7 +2168,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>8</v>
       </c>
@@ -2205,7 +2208,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>8</v>
       </c>
@@ -2245,7 +2248,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>8</v>
       </c>
@@ -2285,7 +2288,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>8</v>
       </c>
@@ -2325,7 +2328,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>8</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>8</v>
       </c>
@@ -2405,7 +2408,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>8</v>
       </c>
@@ -2445,7 +2448,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>8</v>
       </c>
@@ -2485,7 +2488,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>8</v>
       </c>
@@ -2525,7 +2528,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>8</v>
       </c>
@@ -2565,7 +2568,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>8</v>
       </c>
@@ -2605,7 +2608,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>8</v>
       </c>
@@ -2645,7 +2648,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>8</v>
       </c>
@@ -2685,7 +2688,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>8</v>
       </c>
@@ -2725,7 +2728,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>8</v>
       </c>
@@ -2765,7 +2768,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>8</v>
       </c>
@@ -2805,7 +2808,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>8</v>
       </c>
@@ -2845,7 +2848,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>8</v>
       </c>
@@ -2885,7 +2888,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>8</v>
       </c>
@@ -2925,7 +2928,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>8</v>
       </c>
@@ -2965,7 +2968,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>8</v>
       </c>
@@ -3005,7 +3008,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>8</v>
       </c>
@@ -3045,7 +3048,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>8</v>
       </c>
@@ -3085,7 +3088,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>8</v>
       </c>
@@ -3125,7 +3128,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>8</v>
       </c>
@@ -3165,7 +3168,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>8</v>
       </c>
@@ -3205,7 +3208,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>8</v>
       </c>
@@ -3245,7 +3248,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>8</v>
       </c>
@@ -3285,7 +3288,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>8</v>
       </c>
@@ -3325,7 +3328,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>8</v>
       </c>
@@ -3365,7 +3368,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>8</v>
       </c>
@@ -3405,7 +3408,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>8</v>
       </c>
@@ -3445,7 +3448,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>8</v>
       </c>
@@ -3485,7 +3488,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>8</v>
       </c>
@@ -3525,7 +3528,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>8</v>
       </c>
@@ -3565,7 +3568,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>8</v>
       </c>
@@ -3605,7 +3608,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>8</v>
       </c>
@@ -3645,7 +3648,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>8</v>
       </c>
@@ -3685,7 +3688,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>8</v>
       </c>
@@ -3725,7 +3728,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>8</v>
       </c>
@@ -3765,7 +3768,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>8</v>
       </c>
@@ -3805,7 +3808,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>8</v>
       </c>
@@ -3845,7 +3848,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>8</v>
       </c>
@@ -3885,7 +3888,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>8</v>
       </c>
@@ -3925,7 +3928,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>8</v>
       </c>
@@ -3965,7 +3968,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>8</v>
       </c>
@@ -4005,7 +4008,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>8</v>
       </c>
@@ -4045,7 +4048,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>8</v>
       </c>
@@ -4085,7 +4088,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>8</v>
       </c>
@@ -4125,7 +4128,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>8</v>
       </c>
@@ -4165,7 +4168,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>8</v>
       </c>
@@ -4205,7 +4208,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>8</v>
       </c>
@@ -4245,7 +4248,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>8</v>
       </c>
@@ -4285,7 +4288,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>8</v>
       </c>
@@ -4325,7 +4328,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>8</v>
       </c>
@@ -4365,7 +4368,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>8</v>
       </c>
@@ -4405,7 +4408,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>8</v>
       </c>
@@ -4445,7 +4448,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>8</v>
       </c>
@@ -4485,7 +4488,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>8</v>
       </c>
@@ -4525,7 +4528,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>8</v>
       </c>
@@ -4565,7 +4568,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>8</v>
       </c>
@@ -4605,7 +4608,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>8</v>
       </c>
@@ -4645,7 +4648,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>8</v>
       </c>
@@ -4685,7 +4688,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>8</v>
       </c>
@@ -4725,7 +4728,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>8</v>
       </c>
@@ -4765,7 +4768,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>8</v>
       </c>
@@ -4805,7 +4808,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>8</v>
       </c>
@@ -4845,7 +4848,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>8</v>
       </c>
@@ -4885,7 +4888,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>8</v>
       </c>
@@ -4925,7 +4928,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>8</v>
       </c>
@@ -4965,7 +4968,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>8</v>
       </c>
@@ -5005,7 +5008,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>8</v>
       </c>
@@ -5045,7 +5048,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>8</v>
       </c>
@@ -5085,7 +5088,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>8</v>
       </c>
@@ -5125,7 +5128,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>8</v>
       </c>
@@ -5165,7 +5168,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>8</v>
       </c>
@@ -5205,7 +5208,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>8</v>
       </c>
@@ -5245,7 +5248,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>8</v>
       </c>
@@ -5285,7 +5288,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>8</v>
       </c>
@@ -5325,7 +5328,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>8</v>
       </c>
@@ -5365,7 +5368,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>8</v>
       </c>
@@ -5405,7 +5408,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>8</v>
       </c>
@@ -5445,7 +5448,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>8</v>
       </c>
@@ -5485,7 +5488,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>8</v>
       </c>
@@ -5525,7 +5528,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>8</v>
       </c>
@@ -5565,7 +5568,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>8</v>
       </c>
@@ -5605,7 +5608,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>8</v>
       </c>
@@ -5645,7 +5648,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>8</v>
       </c>
@@ -5685,7 +5688,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>8</v>
       </c>
@@ -5725,7 +5728,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>8</v>
       </c>
@@ -5765,7 +5768,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>8</v>
       </c>
@@ -5805,7 +5808,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>8</v>
       </c>
@@ -5845,7 +5848,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>8</v>
       </c>
@@ -5885,7 +5888,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>8</v>
       </c>
@@ -5925,7 +5928,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>8</v>
       </c>
@@ -5965,7 +5968,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>8</v>
       </c>
@@ -6005,7 +6008,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>8</v>
       </c>
@@ -6045,7 +6048,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>8</v>
       </c>
@@ -6085,7 +6088,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>8</v>
       </c>
@@ -6125,7 +6128,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>8</v>
       </c>
@@ -6165,7 +6168,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>8</v>
       </c>
@@ -6205,7 +6208,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>8</v>
       </c>
@@ -6245,7 +6248,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>8</v>
       </c>
@@ -6285,7 +6288,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>8</v>
       </c>
@@ -6325,7 +6328,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>8</v>
       </c>
@@ -6365,7 +6368,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>8</v>
       </c>
@@ -6405,7 +6408,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>8</v>
       </c>
@@ -6445,7 +6448,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>8</v>
       </c>
@@ -6485,7 +6488,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>8</v>
       </c>
@@ -6525,7 +6528,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>8</v>
       </c>
@@ -6565,7 +6568,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>8</v>
       </c>
@@ -6605,7 +6608,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>8</v>
       </c>
@@ -6645,7 +6648,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>8</v>
       </c>
@@ -6685,7 +6688,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>8</v>
       </c>
@@ -6725,7 +6728,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>8</v>
       </c>
@@ -6765,7 +6768,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>8</v>
       </c>
@@ -6805,7 +6808,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>8</v>
       </c>
@@ -6845,7 +6848,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>8</v>
       </c>
@@ -6885,7 +6888,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>8</v>
       </c>
@@ -6925,7 +6928,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
         <v>8</v>
       </c>
@@ -6965,7 +6968,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>8</v>
       </c>
@@ -7005,7 +7008,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>8</v>
       </c>
@@ -7045,7 +7048,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>8</v>
       </c>
@@ -7085,7 +7088,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>8</v>
       </c>
@@ -7125,7 +7128,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>8</v>
       </c>
@@ -7165,7 +7168,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
         <v>8</v>
       </c>
@@ -7205,7 +7208,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>8</v>
       </c>
@@ -7245,7 +7248,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
         <v>8</v>
       </c>
@@ -7285,7 +7288,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>8</v>
       </c>
@@ -7325,7 +7328,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>8</v>
       </c>
@@ -7365,7 +7368,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>8</v>
       </c>
@@ -7405,7 +7408,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>8</v>
       </c>
@@ -7445,7 +7448,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
         <v>8</v>
       </c>
@@ -7485,7 +7488,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
         <v>8</v>
       </c>
@@ -7525,7 +7528,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
         <v>8</v>
       </c>
@@ -7565,7 +7568,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>8</v>
       </c>
@@ -7605,7 +7608,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
         <v>8</v>
       </c>
@@ -7645,7 +7648,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
         <v>8</v>
       </c>
@@ -7685,7 +7688,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
         <v>8</v>
       </c>
@@ -7725,7 +7728,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
         <v>8</v>
       </c>
@@ -7765,7 +7768,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
         <v>8</v>
       </c>
@@ -7805,7 +7808,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
         <v>8</v>
       </c>
@@ -7845,7 +7848,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
         <v>8</v>
       </c>
@@ -7885,7 +7888,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
         <v>8</v>
       </c>
@@ -7925,7 +7928,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="6" t="s">
         <v>8</v>
       </c>
@@ -7965,7 +7968,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="6" t="s">
         <v>8</v>
       </c>
@@ -8005,7 +8008,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
         <v>8</v>
       </c>
@@ -8045,7 +8048,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
         <v>8</v>
       </c>
@@ -8085,7 +8088,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
         <v>8</v>
       </c>
@@ -8125,7 +8128,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
         <v>8</v>
       </c>
@@ -8165,7 +8168,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
         <v>8</v>
       </c>
@@ -8205,7 +8208,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
         <v>8</v>
       </c>
@@ -8245,7 +8248,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
         <v>8</v>
       </c>
@@ -8285,7 +8288,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
         <v>8</v>
       </c>
@@ -8325,7 +8328,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
         <v>8</v>
       </c>
@@ -8365,7 +8368,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
         <v>8</v>
       </c>
@@ -8405,7 +8408,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
         <v>8</v>
       </c>
@@ -8445,7 +8448,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
         <v>8</v>
       </c>
@@ -8485,7 +8488,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
         <v>8</v>
       </c>
@@ -8525,7 +8528,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
         <v>8</v>
       </c>
@@ -8565,7 +8568,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
         <v>8</v>
       </c>
@@ -8605,7 +8608,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
         <v>8</v>
       </c>
@@ -8645,7 +8648,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
         <v>8</v>
       </c>
@@ -8685,7 +8688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
         <v>8</v>
       </c>
@@ -8725,7 +8728,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
         <v>8</v>
       </c>
@@ -8765,7 +8768,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="6" t="s">
         <v>8</v>
       </c>
@@ -8805,7 +8808,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="6" t="s">
         <v>8</v>
       </c>
@@ -8845,7 +8848,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="6" t="s">
         <v>8</v>
       </c>
@@ -8885,7 +8888,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="6" t="s">
         <v>8</v>
       </c>
@@ -8925,7 +8928,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="6" t="s">
         <v>8</v>
       </c>
@@ -8965,7 +8968,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="6" t="s">
         <v>8</v>
       </c>
@@ -9005,7 +9008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="6" t="s">
         <v>8</v>
       </c>
@@ -9045,7 +9048,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="6" t="s">
         <v>8</v>
       </c>
@@ -9085,7 +9088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="6" t="s">
         <v>8</v>
       </c>
@@ -9125,7 +9128,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="6" t="s">
         <v>8</v>
       </c>
@@ -9165,7 +9168,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="6" t="s">
         <v>8</v>
       </c>
@@ -9205,7 +9208,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="6" t="s">
         <v>8</v>
       </c>
@@ -9245,7 +9248,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="6" t="s">
         <v>8</v>
       </c>
@@ -9285,7 +9288,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="6" t="s">
         <v>8</v>
       </c>
@@ -9325,7 +9328,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="6" t="s">
         <v>8</v>
       </c>
@@ -9365,7 +9368,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="6" t="s">
         <v>8</v>
       </c>
@@ -9405,7 +9408,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="6" t="s">
         <v>8</v>
       </c>
@@ -9445,7 +9448,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="6" t="s">
         <v>8</v>
       </c>
@@ -9485,7 +9488,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="6" t="s">
         <v>8</v>
       </c>
@@ -9525,7 +9528,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="6" t="s">
         <v>8</v>
       </c>
@@ -9565,7 +9568,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="6" t="s">
         <v>8</v>
       </c>
@@ -9605,7 +9608,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="6" t="s">
         <v>8</v>
       </c>
@@ -9645,7 +9648,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="6" t="s">
         <v>8</v>
       </c>
@@ -9685,7 +9688,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="6" t="s">
         <v>8</v>
       </c>
@@ -9725,7 +9728,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="6" t="s">
         <v>8</v>
       </c>
@@ -9765,7 +9768,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="6" t="s">
         <v>8</v>
       </c>
@@ -9805,7 +9808,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="6" t="s">
         <v>8</v>
       </c>
@@ -9845,7 +9848,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="6" t="s">
         <v>8</v>
       </c>
@@ -9885,7 +9888,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="6" t="s">
         <v>8</v>
       </c>
@@ -9925,7 +9928,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="6" t="s">
         <v>8</v>
       </c>
@@ -9965,7 +9968,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="6" t="s">
         <v>8</v>
       </c>
@@ -10005,7 +10008,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="6" t="s">
         <v>8</v>
       </c>
@@ -10045,7 +10048,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="6" t="s">
         <v>8</v>
       </c>
@@ -10085,7 +10088,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="6" t="s">
         <v>8</v>
       </c>
@@ -10125,7 +10128,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="6" t="s">
         <v>8</v>
       </c>
@@ -10165,7 +10168,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="6" t="s">
         <v>8</v>
       </c>
@@ -10205,7 +10208,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
         <v>8</v>
       </c>
@@ -10245,7 +10248,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
         <v>8</v>
       </c>
@@ -10285,7 +10288,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="6" t="s">
         <v>8</v>
       </c>
@@ -10325,7 +10328,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
         <v>8</v>
       </c>
@@ -10365,7 +10368,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="6" t="s">
         <v>8</v>
       </c>
@@ -10405,7 +10408,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="6" t="s">
         <v>8</v>
       </c>
@@ -10445,7 +10448,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
         <v>8</v>
       </c>
@@ -10485,7 +10488,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="6" t="s">
         <v>8</v>
       </c>
@@ -10525,7 +10528,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="6" t="s">
         <v>8</v>
       </c>
@@ -10565,7 +10568,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
         <v>8</v>
       </c>
@@ -10605,7 +10608,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="6" t="s">
         <v>8</v>
       </c>
@@ -10645,7 +10648,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="6" t="s">
         <v>8</v>
       </c>
@@ -10685,7 +10688,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="6" t="s">
         <v>8</v>
       </c>
@@ -10725,7 +10728,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="6" t="s">
         <v>8</v>
       </c>
@@ -10765,7 +10768,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="6" t="s">
         <v>8</v>
       </c>
@@ -10805,7 +10808,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="6" t="s">
         <v>8</v>
       </c>
@@ -10845,7 +10848,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="6" t="s">
         <v>8</v>
       </c>
@@ -10885,7 +10888,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="6" t="s">
         <v>8</v>
       </c>
@@ -10925,7 +10928,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="6" t="s">
         <v>8</v>
       </c>
@@ -10965,7 +10968,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="6" t="s">
         <v>8</v>
       </c>
@@ -11005,7 +11008,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="6" t="s">
         <v>8</v>
       </c>
@@ -11045,7 +11048,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="6" t="s">
         <v>8</v>
       </c>
@@ -11085,7 +11088,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="6" t="s">
         <v>8</v>
       </c>
@@ -11125,7 +11128,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="6" t="s">
         <v>8</v>
       </c>
@@ -11165,7 +11168,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="6" t="s">
         <v>8</v>
       </c>
@@ -11205,7 +11208,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="6" t="s">
         <v>8</v>
       </c>
@@ -11245,7 +11248,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="6" t="s">
         <v>8</v>
       </c>
@@ -11285,7 +11288,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="6" t="s">
         <v>8</v>
       </c>
@@ -11325,7 +11328,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="6" t="s">
         <v>8</v>
       </c>
@@ -11365,7 +11368,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="6" t="s">
         <v>8</v>
       </c>
@@ -11405,7 +11408,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="6" t="s">
         <v>8</v>
       </c>
@@ -11445,7 +11448,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" s="6" t="s">
         <v>8</v>
       </c>
@@ -11485,7 +11488,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" s="6" t="s">
         <v>8</v>
       </c>
@@ -11525,7 +11528,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" s="6" t="s">
         <v>8</v>
       </c>
@@ -11565,7 +11568,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" s="6" t="s">
         <v>8</v>
       </c>
@@ -11605,7 +11608,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="6" t="s">
         <v>8</v>
       </c>
@@ -11645,7 +11648,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" s="6" t="s">
         <v>8</v>
       </c>
@@ -11685,7 +11688,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" s="6" t="s">
         <v>8</v>
       </c>
@@ -11725,7 +11728,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" s="6" t="s">
         <v>8</v>
       </c>
@@ -11765,7 +11768,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="6" t="s">
         <v>8</v>
       </c>
@@ -11805,7 +11808,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" s="6" t="s">
         <v>8</v>
       </c>
@@ -11845,7 +11848,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="6" t="s">
         <v>8</v>
       </c>
@@ -11885,7 +11888,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261" s="6" t="s">
         <v>8</v>
       </c>
@@ -11925,7 +11928,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" s="6" t="s">
         <v>8</v>
       </c>
@@ -11965,7 +11968,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" s="6" t="s">
         <v>8</v>
       </c>
@@ -12005,7 +12008,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" s="6" t="s">
         <v>8</v>
       </c>
@@ -12045,7 +12048,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" s="6" t="s">
         <v>8</v>
       </c>
@@ -12085,7 +12088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" s="6" t="s">
         <v>8</v>
       </c>
@@ -12125,7 +12128,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" s="6" t="s">
         <v>8</v>
       </c>
@@ -12165,7 +12168,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" s="6" t="s">
         <v>8</v>
       </c>
@@ -12205,7 +12208,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="6" t="s">
         <v>8</v>
       </c>
@@ -12245,7 +12248,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" s="6" t="s">
         <v>8</v>
       </c>
@@ -12285,7 +12288,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" s="6" t="s">
         <v>8</v>
       </c>
@@ -12325,7 +12328,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="6" t="s">
         <v>8</v>
       </c>
@@ -12365,7 +12368,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" s="6" t="s">
         <v>8</v>
       </c>
@@ -12405,7 +12408,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" s="6" t="s">
         <v>8</v>
       </c>
@@ -12445,7 +12448,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" s="6" t="s">
         <v>8</v>
       </c>
@@ -12485,7 +12488,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" s="6" t="s">
         <v>8</v>
       </c>
@@ -12525,7 +12528,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" s="6" t="s">
         <v>8</v>
       </c>
@@ -12565,7 +12568,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="6" t="s">
         <v>8</v>
       </c>
@@ -12605,7 +12608,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="6" t="s">
         <v>8</v>
       </c>
@@ -12645,7 +12648,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" s="6" t="s">
         <v>8</v>
       </c>
@@ -12685,7 +12688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="6" t="s">
         <v>8</v>
       </c>
@@ -12725,7 +12728,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="6" t="s">
         <v>8</v>
       </c>
@@ -12765,7 +12768,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" s="6" t="s">
         <v>8</v>
       </c>
@@ -12805,7 +12808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="6" t="s">
         <v>8</v>
       </c>
@@ -12845,7 +12848,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" s="6" t="s">
         <v>8</v>
       </c>
@@ -12885,7 +12888,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" s="6" t="s">
         <v>8</v>
       </c>
@@ -12925,7 +12928,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" s="6" t="s">
         <v>8</v>
       </c>
@@ -12965,7 +12968,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" s="6" t="s">
         <v>8</v>
       </c>
@@ -13005,7 +13008,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" s="6" t="s">
         <v>8</v>
       </c>
@@ -13045,7 +13048,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" s="6" t="s">
         <v>8</v>
       </c>
@@ -13085,7 +13088,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A291" s="6" t="s">
         <v>8</v>
       </c>
@@ -13125,7 +13128,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A292" s="6" t="s">
         <v>8</v>
       </c>
@@ -13165,7 +13168,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A293" s="6" t="s">
         <v>8</v>
       </c>
@@ -13205,7 +13208,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294" s="6" t="s">
         <v>8</v>
       </c>
@@ -13245,7 +13248,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A295" s="6" t="s">
         <v>8</v>
       </c>
@@ -13285,7 +13288,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296" s="6" t="s">
         <v>8</v>
       </c>
@@ -13325,7 +13328,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A297" s="6" t="s">
         <v>8</v>
       </c>
@@ -13365,7 +13368,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298" s="6" t="s">
         <v>8</v>
       </c>
@@ -13405,7 +13408,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299" s="6" t="s">
         <v>8</v>
       </c>
@@ -13445,7 +13448,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300" s="6" t="s">
         <v>8</v>
       </c>
@@ -13485,7 +13488,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A301" s="6" t="s">
         <v>8</v>
       </c>
@@ -13525,7 +13528,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302" s="6" t="s">
         <v>8</v>
       </c>
@@ -13565,7 +13568,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A303" s="6" t="s">
         <v>8</v>
       </c>
@@ -13605,7 +13608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" s="6" t="s">
         <v>8</v>
       </c>
@@ -13645,7 +13648,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A305" s="6" t="s">
         <v>8</v>
       </c>
@@ -13685,7 +13688,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" s="6" t="s">
         <v>8</v>
       </c>
@@ -13725,7 +13728,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307" s="6" t="s">
         <v>8</v>
       </c>
@@ -13765,7 +13768,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="6" t="s">
         <v>8</v>
       </c>
@@ -13805,7 +13808,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A309" s="6" t="s">
         <v>8</v>
       </c>
@@ -13845,7 +13848,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A310" s="6" t="s">
         <v>8</v>
       </c>
@@ -13885,7 +13888,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A311" s="6" t="s">
         <v>8</v>
       </c>
@@ -13925,7 +13928,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A312" s="6" t="s">
         <v>8</v>
       </c>
@@ -13965,7 +13968,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A313" s="6" t="s">
         <v>8</v>
       </c>
@@ -14005,7 +14008,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A314" s="6" t="s">
         <v>8</v>
       </c>
@@ -14045,7 +14048,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A315" s="6" t="s">
         <v>8</v>
       </c>
@@ -14085,7 +14088,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" s="6" t="s">
         <v>8</v>
       </c>
@@ -14125,7 +14128,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" s="6" t="s">
         <v>8</v>
       </c>
@@ -14165,7 +14168,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="6" t="s">
         <v>8</v>
       </c>
@@ -14205,7 +14208,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319" s="6" t="s">
         <v>8</v>
       </c>
@@ -14245,7 +14248,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A320" s="6" t="s">
         <v>8</v>
       </c>
@@ -14285,7 +14288,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321" s="6" t="s">
         <v>8</v>
       </c>
@@ -14325,7 +14328,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322" s="6" t="s">
         <v>8</v>
       </c>
@@ -14365,7 +14368,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A323" s="6" t="s">
         <v>8</v>
       </c>
@@ -14405,7 +14408,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" s="6" t="s">
         <v>8</v>
       </c>
@@ -14445,7 +14448,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325" s="6" t="s">
         <v>8</v>
       </c>
@@ -14485,7 +14488,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326" s="6" t="s">
         <v>8</v>
       </c>
@@ -14525,7 +14528,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" s="6" t="s">
         <v>8</v>
       </c>
@@ -14565,7 +14568,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328" s="6" t="s">
         <v>8</v>
       </c>
@@ -14605,7 +14608,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329" s="6" t="s">
         <v>8</v>
       </c>
@@ -14645,7 +14648,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330" s="6" t="s">
         <v>8</v>
       </c>
@@ -14685,7 +14688,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" s="6" t="s">
         <v>8</v>
       </c>
@@ -14725,7 +14728,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332" s="6" t="s">
         <v>8</v>
       </c>
@@ -14765,7 +14768,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333" s="6" t="s">
         <v>8</v>
       </c>
@@ -14805,7 +14808,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334" s="6" t="s">
         <v>8</v>
       </c>
@@ -14845,7 +14848,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335" s="6" t="s">
         <v>8</v>
       </c>
@@ -14885,7 +14888,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336" s="6" t="s">
         <v>8</v>
       </c>
@@ -14925,7 +14928,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337" s="6" t="s">
         <v>8</v>
       </c>
@@ -14965,7 +14968,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338" s="6" t="s">
         <v>8</v>
       </c>
@@ -15005,7 +15008,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339" s="6" t="s">
         <v>8</v>
       </c>
@@ -15045,7 +15048,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340" s="6" t="s">
         <v>8</v>
       </c>
@@ -15085,7 +15088,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341" s="6" t="s">
         <v>8</v>
       </c>
@@ -15125,7 +15128,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" s="6" t="s">
         <v>8</v>
       </c>
@@ -15165,7 +15168,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" s="6" t="s">
         <v>8</v>
       </c>
@@ -15205,7 +15208,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A344" s="6" t="s">
         <v>8</v>
       </c>
@@ -15245,7 +15248,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345" s="6" t="s">
         <v>8</v>
       </c>
@@ -15285,7 +15288,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A346" s="6" t="s">
         <v>8</v>
       </c>
@@ -15325,7 +15328,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A347" s="6" t="s">
         <v>8</v>
       </c>
@@ -15365,7 +15368,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A348" s="6" t="s">
         <v>8</v>
       </c>
@@ -15405,7 +15408,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349" s="6" t="s">
         <v>8</v>
       </c>
@@ -15445,7 +15448,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A350" s="6" t="s">
         <v>8</v>
       </c>
@@ -15485,7 +15488,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A351" s="6" t="s">
         <v>8</v>
       </c>
@@ -15525,7 +15528,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A352" s="6" t="s">
         <v>8</v>
       </c>
@@ -15565,7 +15568,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A353" s="6" t="s">
         <v>8</v>
       </c>
@@ -15605,7 +15608,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" s="6" t="s">
         <v>8</v>
       </c>
@@ -15645,7 +15648,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355" s="6" t="s">
         <v>8</v>
       </c>
@@ -15685,7 +15688,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A356" s="6" t="s">
         <v>8</v>
       </c>
@@ -15725,7 +15728,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A357" s="6" t="s">
         <v>8</v>
       </c>
@@ -15765,7 +15768,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A358" s="6" t="s">
         <v>8</v>
       </c>
@@ -15805,7 +15808,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A359" s="6" t="s">
         <v>8</v>
       </c>
@@ -15845,7 +15848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A360" s="6" t="s">
         <v>8</v>
       </c>
@@ -15885,7 +15888,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A361" s="6" t="s">
         <v>8</v>
       </c>
@@ -15925,7 +15928,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A362" s="6" t="s">
         <v>8</v>
       </c>
@@ -15965,7 +15968,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A363" s="6" t="s">
         <v>8</v>
       </c>
@@ -16005,7 +16008,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A364" s="6" t="s">
         <v>8</v>
       </c>
@@ -16045,7 +16048,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A365" s="6" t="s">
         <v>8</v>
       </c>
@@ -16085,7 +16088,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366" s="6" t="s">
         <v>8</v>
       </c>
@@ -16125,7 +16128,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A367" s="6" t="s">
         <v>8</v>
       </c>
@@ -16165,7 +16168,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A368" s="6" t="s">
         <v>8</v>
       </c>
@@ -16205,7 +16208,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A369" s="6" t="s">
         <v>8</v>
       </c>
@@ -16245,7 +16248,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A370" s="6" t="s">
         <v>8</v>
       </c>
@@ -16285,7 +16288,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A371" s="6" t="s">
         <v>8</v>
       </c>
@@ -16325,7 +16328,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A372" s="6" t="s">
         <v>8</v>
       </c>
@@ -16365,7 +16368,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A373" s="6" t="s">
         <v>8</v>
       </c>
@@ -16405,7 +16408,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" s="6" t="s">
         <v>8</v>
       </c>
@@ -16445,7 +16448,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A375" s="6" t="s">
         <v>8</v>
       </c>
@@ -16485,7 +16488,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A376" s="6" t="s">
         <v>8</v>
       </c>
@@ -16525,7 +16528,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377" s="6" t="s">
         <v>8</v>
       </c>
@@ -16565,7 +16568,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A378" s="6" t="s">
         <v>8</v>
       </c>
@@ -16605,7 +16608,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" s="6" t="s">
         <v>8</v>
       </c>
@@ -16645,7 +16648,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" s="6" t="s">
         <v>8</v>
       </c>
@@ -16685,7 +16688,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A381" s="6" t="s">
         <v>8</v>
       </c>
@@ -16725,7 +16728,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A382" s="6" t="s">
         <v>8</v>
       </c>
@@ -16765,7 +16768,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A383" s="6" t="s">
         <v>8</v>
       </c>
@@ -16805,7 +16808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A384" s="6" t="s">
         <v>8</v>
       </c>
@@ -16845,7 +16848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A385" s="6" t="s">
         <v>8</v>
       </c>
@@ -16885,7 +16888,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A386" s="6" t="s">
         <v>8</v>
       </c>
@@ -16925,7 +16928,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A387" s="6" t="s">
         <v>8</v>
       </c>
@@ -16965,7 +16968,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A388" s="6" t="s">
         <v>8</v>
       </c>
@@ -17005,7 +17008,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A389" s="6" t="s">
         <v>8</v>
       </c>
@@ -17045,7 +17048,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A390" s="6" t="s">
         <v>8</v>
       </c>
@@ -17085,7 +17088,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A391" s="6" t="s">
         <v>8</v>
       </c>
@@ -17125,7 +17128,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A392" s="6" t="s">
         <v>8</v>
       </c>
@@ -17165,7 +17168,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A393" s="6" t="s">
         <v>8</v>
       </c>
@@ -17205,63 +17208,82 @@
         <v>286</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A394" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C394" s="2"/>
-      <c r="D394" s="1"/>
-      <c r="E394" s="2"/>
+      <c r="B394" s="1">
+        <v>45595</v>
+      </c>
+      <c r="C394" s="2">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D394" s="1">
+        <v>45596</v>
+      </c>
+      <c r="E394" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F394" s="3">
         <f>INT(Table1[[#This Row],[Start Date]])</f>
-        <v>0</v>
+        <v>45595</v>
       </c>
       <c r="G394" s="3">
         <f>INT(Table1[[#This Row],[End Date]])</f>
-        <v>0</v>
+        <v>45596</v>
       </c>
       <c r="H394" s="3">
         <f>(_xlfn.DAYS(Table1[[#This Row],[End Date]],Table1[[#This Row],[Start Date]]) + Table1[[#This Row],[End Time]] - Table1[[#This Row],[Start Time]]) * 24</f>
-        <v>0</v>
-      </c>
-      <c r="I394" s="13" t="str">
+        <v>2.0000000000000009</v>
+      </c>
+      <c r="I394" s="13">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="J394" s="4" t="str">
-        <f>IF(Table1[[#This Row],[Elapsed Hours Raw]]&gt;0,Table1[[#This Row],[Elapsed Hours Raw]],IF(Table1[[#This Row],[Elapsed Hours Raw]]&lt;0,"…",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J394" s="4">
+        <f>IF(Table1[[#This Row],[Elapsed Hours Raw]]&gt;0,Table1[[#This Row],[Elapsed Hours Raw]],IF(Table1[[#This Row],[Elapsed Hours Raw]]&lt;0,"…",""))</f>
+        <v>2.0000000000000009</v>
+      </c>
+      <c r="K394" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A395" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C395" s="2"/>
-      <c r="D395" s="1"/>
+      <c r="B395" s="1">
+        <v>45596</v>
+      </c>
+      <c r="C395" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D395" s="1">
+        <v>45596</v>
+      </c>
       <c r="E395" s="2"/>
       <c r="F395" s="3">
         <f>INT(Table1[[#This Row],[Start Date]])</f>
-        <v>0</v>
+        <v>45596</v>
       </c>
       <c r="G395" s="3">
         <f>INT(Table1[[#This Row],[End Date]])</f>
-        <v>0</v>
+        <v>45596</v>
       </c>
       <c r="H395" s="3">
         <f>(_xlfn.DAYS(Table1[[#This Row],[End Date]],Table1[[#This Row],[Start Date]]) + Table1[[#This Row],[End Time]] - Table1[[#This Row],[Start Time]]) * 24</f>
-        <v>0</v>
-      </c>
-      <c r="I395" s="13" t="str">
+        <v>-15.5</v>
+      </c>
+      <c r="I395" s="13">
         <f t="shared" si="6"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="J395" s="4" t="str">
         <f>IF(Table1[[#This Row],[Elapsed Hours Raw]]&gt;0,Table1[[#This Row],[Elapsed Hours Raw]],IF(Table1[[#This Row],[Elapsed Hours Raw]]&lt;0,"…",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="396" spans="1:11" x14ac:dyDescent="0.3">
+        <v>…</v>
+      </c>
+    </row>
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A396" s="6" t="s">
         <v>8</v>
       </c>
@@ -17289,7 +17311,7 @@
         <v/>
       </c>
     </row>
-    <row r="397" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A397" s="6" t="s">
         <v>8</v>
       </c>
@@ -17317,7 +17339,7 @@
         <v/>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A398" s="6" t="s">
         <v>8</v>
       </c>
@@ -17345,7 +17367,7 @@
         <v/>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A399" s="6" t="s">
         <v>8</v>
       </c>
@@ -17373,7 +17395,7 @@
         <v/>
       </c>
     </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A400" s="6" t="s">
         <v>8</v>
       </c>
@@ -17401,7 +17423,7 @@
         <v/>
       </c>
     </row>
-    <row r="401" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A401" s="6" t="s">
         <v>8</v>
       </c>
@@ -17429,7 +17451,7 @@
         <v/>
       </c>
     </row>
-    <row r="402" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A402" s="6" t="s">
         <v>8</v>
       </c>
@@ -17457,7 +17479,7 @@
         <v/>
       </c>
     </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A403" s="6" t="s">
         <v>8</v>
       </c>
@@ -17485,7 +17507,7 @@
         <v/>
       </c>
     </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A404" s="6" t="s">
         <v>8</v>
       </c>
@@ -17513,7 +17535,7 @@
         <v/>
       </c>
     </row>
-    <row r="405" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A405" s="6" t="s">
         <v>8</v>
       </c>
@@ -17541,7 +17563,7 @@
         <v/>
       </c>
     </row>
-    <row r="406" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A406" s="6" t="s">
         <v>8</v>
       </c>
@@ -17569,7 +17591,7 @@
         <v/>
       </c>
     </row>
-    <row r="407" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A407" s="6" t="s">
         <v>8</v>
       </c>
@@ -17597,7 +17619,7 @@
         <v/>
       </c>
     </row>
-    <row r="408" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A408" s="6" t="s">
         <v>8</v>
       </c>
@@ -17625,7 +17647,7 @@
         <v/>
       </c>
     </row>
-    <row r="409" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A409" s="6" t="s">
         <v>8</v>
       </c>
@@ -17653,7 +17675,7 @@
         <v/>
       </c>
     </row>
-    <row r="410" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A410" s="6" t="s">
         <v>8</v>
       </c>
@@ -17681,7 +17703,7 @@
         <v/>
       </c>
     </row>
-    <row r="411" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A411" s="6" t="s">
         <v>8</v>
       </c>
@@ -17709,7 +17731,7 @@
         <v/>
       </c>
     </row>
-    <row r="412" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A412" s="6" t="s">
         <v>8</v>
       </c>
@@ -17737,7 +17759,7 @@
         <v/>
       </c>
     </row>
-    <row r="413" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A413" s="6" t="s">
         <v>8</v>
       </c>
@@ -17765,7 +17787,7 @@
         <v/>
       </c>
     </row>
-    <row r="414" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A414" s="6" t="s">
         <v>8</v>
       </c>
@@ -17793,7 +17815,7 @@
         <v/>
       </c>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A415" s="6" t="s">
         <v>8</v>
       </c>
@@ -17821,7 +17843,7 @@
         <v/>
       </c>
     </row>
-    <row r="416" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A416" s="6" t="s">
         <v>8</v>
       </c>
@@ -17849,7 +17871,7 @@
         <v/>
       </c>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A417" s="6" t="s">
         <v>8</v>
       </c>
@@ -17877,7 +17899,7 @@
         <v/>
       </c>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A418" s="6" t="s">
         <v>8</v>
       </c>
@@ -17905,7 +17927,7 @@
         <v/>
       </c>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A419" s="6" t="s">
         <v>8</v>
       </c>
@@ -17933,7 +17955,7 @@
         <v/>
       </c>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A420" s="6" t="s">
         <v>8</v>
       </c>
@@ -17961,7 +17983,7 @@
         <v/>
       </c>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A421" s="6" t="s">
         <v>8</v>
       </c>
@@ -17989,7 +18011,7 @@
         <v/>
       </c>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A422" s="6" t="s">
         <v>8</v>
       </c>
@@ -18017,7 +18039,7 @@
         <v/>
       </c>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A423" s="6" t="s">
         <v>8</v>
       </c>
@@ -18045,7 +18067,7 @@
         <v/>
       </c>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A424" s="6" t="s">
         <v>8</v>
       </c>
@@ -18073,7 +18095,7 @@
         <v/>
       </c>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A425" s="6" t="s">
         <v>8</v>
       </c>
@@ -18101,7 +18123,7 @@
         <v/>
       </c>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A426" s="6" t="s">
         <v>8</v>
       </c>
@@ -18129,7 +18151,7 @@
         <v/>
       </c>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A427" s="6" t="s">
         <v>8</v>
       </c>
@@ -18157,7 +18179,7 @@
         <v/>
       </c>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A428" s="6" t="s">
         <v>8</v>
       </c>
@@ -18185,7 +18207,7 @@
         <v/>
       </c>
     </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A429" s="6" t="s">
         <v>8</v>
       </c>
@@ -18213,7 +18235,7 @@
         <v/>
       </c>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A430" s="6" t="s">
         <v>8</v>
       </c>
@@ -18241,7 +18263,7 @@
         <v/>
       </c>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A431" s="6" t="s">
         <v>8</v>
       </c>
@@ -18269,7 +18291,7 @@
         <v/>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A432" s="6" t="s">
         <v>8</v>
       </c>
@@ -18297,7 +18319,7 @@
         <v/>
       </c>
     </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A433" s="6" t="s">
         <v>8</v>
       </c>
@@ -18325,7 +18347,7 @@
         <v/>
       </c>
     </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A434" s="6" t="s">
         <v>8</v>
       </c>
@@ -18353,7 +18375,7 @@
         <v/>
       </c>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A435" s="6" t="s">
         <v>8</v>
       </c>
@@ -18381,7 +18403,7 @@
         <v/>
       </c>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A436" s="6" t="s">
         <v>8</v>
       </c>
@@ -18409,7 +18431,7 @@
         <v/>
       </c>
     </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A437" s="6" t="s">
         <v>8</v>
       </c>
@@ -18437,7 +18459,7 @@
         <v/>
       </c>
     </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A438" s="6" t="s">
         <v>8</v>
       </c>
@@ -18465,7 +18487,7 @@
         <v/>
       </c>
     </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A439" s="6" t="s">
         <v>8</v>
       </c>
@@ -18493,7 +18515,7 @@
         <v/>
       </c>
     </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A440" s="6" t="s">
         <v>8</v>
       </c>
@@ -18521,7 +18543,7 @@
         <v/>
       </c>
     </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A441" s="6" t="s">
         <v>8</v>
       </c>
@@ -18549,7 +18571,7 @@
         <v/>
       </c>
     </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A442" s="6" t="s">
         <v>8</v>
       </c>
@@ -18577,7 +18599,7 @@
         <v/>
       </c>
     </row>
-    <row r="443" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A443" s="6" t="s">
         <v>8</v>
       </c>
@@ -18605,7 +18627,7 @@
         <v/>
       </c>
     </row>
-    <row r="444" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A444" s="6" t="s">
         <v>8</v>
       </c>
@@ -18633,7 +18655,7 @@
         <v/>
       </c>
     </row>
-    <row r="445" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A445" s="6" t="s">
         <v>8</v>
       </c>
@@ -18661,7 +18683,7 @@
         <v/>
       </c>
     </row>
-    <row r="446" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A446" s="6" t="s">
         <v>8</v>
       </c>
@@ -18689,7 +18711,7 @@
         <v/>
       </c>
     </row>
-    <row r="447" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A447" s="6" t="s">
         <v>8</v>
       </c>
@@ -18717,7 +18739,7 @@
         <v/>
       </c>
     </row>
-    <row r="448" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A448" s="6" t="s">
         <v>8</v>
       </c>
@@ -18745,7 +18767,7 @@
         <v/>
       </c>
     </row>
-    <row r="449" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A449" s="6" t="s">
         <v>8</v>
       </c>
@@ -18773,7 +18795,7 @@
         <v/>
       </c>
     </row>
-    <row r="450" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A450" s="6" t="s">
         <v>8</v>
       </c>
@@ -18801,7 +18823,7 @@
         <v/>
       </c>
     </row>
-    <row r="451" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A451" s="6" t="s">
         <v>8</v>
       </c>
@@ -18829,7 +18851,7 @@
         <v/>
       </c>
     </row>
-    <row r="452" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A452" s="6" t="s">
         <v>8</v>
       </c>
@@ -18857,7 +18879,7 @@
         <v/>
       </c>
     </row>
-    <row r="453" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A453" s="6" t="s">
         <v>8</v>
       </c>
@@ -18885,7 +18907,7 @@
         <v/>
       </c>
     </row>
-    <row r="454" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A454" s="6" t="s">
         <v>8</v>
       </c>
@@ -18913,7 +18935,7 @@
         <v/>
       </c>
     </row>
-    <row r="455" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A455" s="6" t="s">
         <v>8</v>
       </c>
@@ -18941,7 +18963,7 @@
         <v/>
       </c>
     </row>
-    <row r="456" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A456" s="6" t="s">
         <v>8</v>
       </c>
@@ -18969,7 +18991,7 @@
         <v/>
       </c>
     </row>
-    <row r="457" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A457" s="6" t="s">
         <v>8</v>
       </c>
@@ -18997,7 +19019,7 @@
         <v/>
       </c>
     </row>
-    <row r="458" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A458" s="6" t="s">
         <v>8</v>
       </c>
@@ -19025,7 +19047,7 @@
         <v/>
       </c>
     </row>
-    <row r="459" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A459" s="6" t="s">
         <v>8</v>
       </c>
@@ -19053,7 +19075,7 @@
         <v/>
       </c>
     </row>
-    <row r="460" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A460" s="6" t="s">
         <v>8</v>
       </c>
@@ -19081,7 +19103,7 @@
         <v/>
       </c>
     </row>
-    <row r="461" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A461" s="6" t="s">
         <v>8</v>
       </c>
@@ -19109,7 +19131,7 @@
         <v/>
       </c>
     </row>
-    <row r="462" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A462" s="6" t="s">
         <v>8</v>
       </c>
@@ -19137,7 +19159,7 @@
         <v/>
       </c>
     </row>
-    <row r="463" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A463" s="6" t="s">
         <v>8</v>
       </c>
@@ -19165,7 +19187,7 @@
         <v/>
       </c>
     </row>
-    <row r="464" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A464" s="6" t="s">
         <v>8</v>
       </c>
@@ -19193,7 +19215,7 @@
         <v/>
       </c>
     </row>
-    <row r="465" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A465" s="6" t="s">
         <v>8</v>
       </c>
@@ -19221,7 +19243,7 @@
         <v/>
       </c>
     </row>
-    <row r="466" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A466" s="6" t="s">
         <v>8</v>
       </c>
@@ -19249,7 +19271,7 @@
         <v/>
       </c>
     </row>
-    <row r="467" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A467" s="6" t="s">
         <v>8</v>
       </c>
@@ -19277,7 +19299,7 @@
         <v/>
       </c>
     </row>
-    <row r="468" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A468" s="6" t="s">
         <v>8</v>
       </c>
@@ -19305,7 +19327,7 @@
         <v/>
       </c>
     </row>
-    <row r="469" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A469" s="6" t="s">
         <v>8</v>
       </c>
@@ -19333,7 +19355,7 @@
         <v/>
       </c>
     </row>
-    <row r="470" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A470" s="6" t="s">
         <v>8</v>
       </c>
@@ -19361,7 +19383,7 @@
         <v/>
       </c>
     </row>
-    <row r="471" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A471" s="6" t="s">
         <v>8</v>
       </c>
@@ -19389,7 +19411,7 @@
         <v/>
       </c>
     </row>
-    <row r="472" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A472" s="6" t="s">
         <v>8</v>
       </c>
@@ -19417,7 +19439,7 @@
         <v/>
       </c>
     </row>
-    <row r="473" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A473" s="6" t="s">
         <v>8</v>
       </c>
@@ -19445,7 +19467,7 @@
         <v/>
       </c>
     </row>
-    <row r="474" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A474" s="6" t="s">
         <v>8</v>
       </c>
@@ -19473,7 +19495,7 @@
         <v/>
       </c>
     </row>
-    <row r="475" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A475" s="6" t="s">
         <v>8</v>
       </c>
@@ -19501,7 +19523,7 @@
         <v/>
       </c>
     </row>
-    <row r="476" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A476" s="6" t="s">
         <v>8</v>
       </c>
@@ -19529,7 +19551,7 @@
         <v/>
       </c>
     </row>
-    <row r="477" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A477" s="6" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Redo extensions, add debug errors with loading
</commit_message>
<xml_diff>
--- a/Management/Minty-Engine_Working_Hours.xlsx
+++ b/Management/Minty-Engine_Working_Hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitch\Documents\Source\Repos\Minty-Engine\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529BA0A0-6C1A-4D8A-AD1B-33CD01722CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DF22DB-F05A-4B2A-B198-B0E95E3AE6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D8840A21-015D-4163-9C78-2CDAAC18DA5A}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{D8840A21-015D-4163-9C78-2CDAAC18DA5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="289">
   <si>
     <t>Start Date</t>
   </si>
@@ -1417,7 +1417,7 @@
       </c>
       <c r="B2" s="8">
         <f>SUMIF(Table1[Elapsed Hours], "&gt;0")</f>
-        <v>1043</v>
+        <v>1047.5</v>
       </c>
       <c r="D2" s="8" t="str">
         <f>ROUNDDOWN($B$2/24, 0) &amp; " days"</f>
@@ -1425,11 +1425,11 @@
       </c>
       <c r="E2" s="10" t="str">
         <f>INT(ROUNDDOWN(MOD($B$2, 24), 0)) &amp; " hours"</f>
-        <v>11 hours</v>
+        <v>15 hours</v>
       </c>
       <c r="F2" s="8" t="str">
         <f>INT(ROUNDDOWN(MOD($B$2,1) * 60,0)) &amp; " minutes"</f>
-        <v>0 minutes</v>
+        <v>30 minutes</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="B3" s="10">
         <f ca="1">SUMIF(Table1[Start Date],TODAY(),Table1[Elapsed Hours])</f>
-        <v>0</v>
+        <v>1.0000000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="B4" s="9" cm="1">
         <f t="array" ref="B4">SUMPRODUCT(1/COUNTIF(Table1[[Start Date Value]:[End Date Value]],Table1[[Start Date Value]:[End Date Value]])) - IF(COUNTIF(Table1[[Start Date Value]:[End Date Value]],"&lt;&gt;0")&gt;0,1,0)</f>
-        <v>240.99999999999937</v>
+        <v>242.00000000000108</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="B6" s="9" cm="1">
         <f t="array" ref="B6">_xlfn.XLOOKUP(TRUE,Table1[Streak]&lt;&gt;"",Table1[Streak],,,-1)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1480,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1BE824-2F12-41E9-9B45-9717EA106B41}">
   <dimension ref="A1:K477"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A381" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E395" sqref="E395"/>
+    <sheetView tabSelected="1" topLeftCell="K390" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K396" sqref="K396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17261,7 +17261,9 @@
       <c r="D395" s="1">
         <v>45596</v>
       </c>
-      <c r="E395" s="2"/>
+      <c r="E395" s="2">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F395" s="3">
         <f>INT(Table1[[#This Row],[Start Date]])</f>
         <v>45596</v>
@@ -17272,43 +17274,58 @@
       </c>
       <c r="H395" s="3">
         <f>(_xlfn.DAYS(Table1[[#This Row],[End Date]],Table1[[#This Row],[Start Date]]) + Table1[[#This Row],[End Time]] - Table1[[#This Row],[Start Time]]) * 24</f>
-        <v>-15.5</v>
+        <v>3.4999999999999982</v>
       </c>
       <c r="I395" s="13">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="J395" s="4" t="str">
-        <f>IF(Table1[[#This Row],[Elapsed Hours Raw]]&gt;0,Table1[[#This Row],[Elapsed Hours Raw]],IF(Table1[[#This Row],[Elapsed Hours Raw]]&lt;0,"…",""))</f>
-        <v>…</v>
+      <c r="J395" s="4">
+        <f>IF(Table1[[#This Row],[Elapsed Hours Raw]]&gt;0,Table1[[#This Row],[Elapsed Hours Raw]],IF(Table1[[#This Row],[Elapsed Hours Raw]]&lt;0,"…",""))</f>
+        <v>3.4999999999999982</v>
+      </c>
+      <c r="K395" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A396" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C396" s="2"/>
-      <c r="D396" s="1"/>
-      <c r="E396" s="2"/>
+      <c r="B396" s="1">
+        <v>45597</v>
+      </c>
+      <c r="C396" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D396" s="1">
+        <v>45597</v>
+      </c>
+      <c r="E396" s="2">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="F396" s="3">
         <f>INT(Table1[[#This Row],[Start Date]])</f>
-        <v>0</v>
+        <v>45597</v>
       </c>
       <c r="G396" s="3">
         <f>INT(Table1[[#This Row],[End Date]])</f>
-        <v>0</v>
+        <v>45597</v>
       </c>
       <c r="H396" s="3">
         <f>(_xlfn.DAYS(Table1[[#This Row],[End Date]],Table1[[#This Row],[Start Date]]) + Table1[[#This Row],[End Time]] - Table1[[#This Row],[Start Time]]) * 24</f>
-        <v>0</v>
-      </c>
-      <c r="I396" s="13" t="str">
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="I396" s="13">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="J396" s="4" t="str">
-        <f>IF(Table1[[#This Row],[Elapsed Hours Raw]]&gt;0,Table1[[#This Row],[Elapsed Hours Raw]],IF(Table1[[#This Row],[Elapsed Hours Raw]]&lt;0,"…",""))</f>
-        <v/>
+        <v>3</v>
+      </c>
+      <c r="J396" s="4">
+        <f>IF(Table1[[#This Row],[Elapsed Hours Raw]]&gt;0,Table1[[#This Row],[Elapsed Hours Raw]],IF(Table1[[#This Row],[Elapsed Hours Raw]]&lt;0,"…",""))</f>
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="K396" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="397" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>